<commit_message>
style: ajustar aba Cliente do modelo para formato vertical (por linhas)
</commit_message>
<xml_diff>
--- a/modelo_planilha.xlsx
+++ b/modelo_planilha.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados_Cliente" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cliente" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mercado_Categoria" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mercado_Subcategoria" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,61 +436,21 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Empresa</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Categoria_Principal</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Ticket_Medio</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Margem_Percentual</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Faturamento_3M</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Unidades_3M</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Range_Permitido_Percentual</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Ticket_Custom</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>CAC</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Investimento_Mkt</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Sua Empresa</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sua Empresa</t>
+          <t>Categoria Macro</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -498,26 +458,82 @@
           <t>Calçados</t>
         </is>
       </c>
-      <c r="C2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ticket Médio Geral</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>250</v>
       </c>
-      <c r="D2" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Margem Atual</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>35</v>
       </c>
-      <c r="E2" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Faturamento Médio 3M</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>150000</v>
       </c>
-      <c r="F2" t="n">
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Unidades Médias 3M</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>600</v>
       </c>
-      <c r="G2" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Range Permitido</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ticket Customizado</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CAC</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>45</v>
       </c>
-      <c r="J2" t="n">
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Investimento Mkt</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>15000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
style: transformar modelo de planilha em template Premium com design profissional
</commit_message>
<xml_diff>
--- a/modelo_planilha.xlsx
+++ b/modelo_planilha.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,16 +30,37 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001E3A8A"/>
+        <bgColor rgb="001E3A8A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F3F4F6"/>
+        <bgColor rgb="00F3F4F6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -53,14 +74,33 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00D1D5DB"/>
+      </left>
+      <right style="thin">
+        <color rgb="00D1D5DB"/>
+      </right>
+      <top style="thin">
+        <color rgb="00D1D5DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00D1D5DB"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,113 +467,129 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CONFIGURAÇÃO DO CLIENTE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VALORES DE EXEMPLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Empresa</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Sua Empresa</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Categoria Macro</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Ticket Médio Geral</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" s="3" t="n">
         <v>250</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Margem Atual</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B5" s="3" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Faturamento Médio 3M</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B6" s="3" t="n">
         <v>150000</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Unidades Médias 3M</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" s="3" t="n">
         <v>600</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Range Permitido</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Ticket Customizado</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>CAC</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" s="3" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Investimento Mkt</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B11" s="3" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -555,134 +611,140 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Categoria</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Periodo</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Faturamento</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unidades</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>2025-01</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="3" t="n">
         <v>1000000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="3" t="n">
         <v>4000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>2025-02</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="3" t="n">
         <v>1100000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="3" t="n">
         <v>4400</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>2025-03</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="3" t="n">
         <v>1050000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="3" t="n">
         <v>4200</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>2025-04</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="3" t="n">
         <v>1200000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="3" t="n">
         <v>4800</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>2025-05</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="3" t="n">
         <v>1150000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="3" t="n">
         <v>4600</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>2025-06</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="3" t="n">
         <v>1300000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="3" t="n">
         <v>5200</v>
       </c>
     </row>
@@ -704,307 +766,314 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Categoria_Macro</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Subcategoria</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Periodo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Faturamento</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Unidades</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Tênis</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>2025-01</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="3" t="n">
         <v>500000</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="3" t="n">
         <v>2000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Tênis</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>2025-02</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="3" t="n">
         <v>550000</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="3" t="n">
         <v>2200</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Tênis</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>2025-03</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="3" t="n">
         <v>520000</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="3" t="n">
         <v>2100</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Tênis</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>2025-04</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="3" t="n">
         <v>600000</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="3" t="n">
         <v>2400</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Tênis</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>2025-05</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="3" t="n">
         <v>580000</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="3" t="n">
         <v>2300</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Tênis</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>2025-06</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="3" t="n">
         <v>650000</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="3" t="n">
         <v>2600</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>Sapatos Sociais</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>2025-01</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="3" t="n">
         <v>200000</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="3" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Sapatos Sociais</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>2025-02</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="3" t="n">
         <v>210000</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="3" t="n">
         <v>840</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>Sapatos Sociais</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>2025-03</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="3" t="n">
         <v>190000</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="3" t="n">
         <v>760</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Sapatos Sociais</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>2025-04</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="3" t="n">
         <v>220000</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="3" t="n">
         <v>880</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>Sapatos Sociais</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>2025-05</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="3" t="n">
         <v>215000</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="3" t="n">
         <v>860</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Calçados</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Calçados</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>Sapatos Sociais</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>2025-06</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="3" t="n">
         <v>230000</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="3" t="n">
         <v>920</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: corrigir compatibilidade de leitura do modelo e adicionar formatação R$
</commit_message>
<xml_diff>
--- a/modelo_planilha.xlsx
+++ b/modelo_planilha.xlsx
@@ -18,7 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <name val="Calibri"/>
@@ -92,13 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -521,7 +524,7 @@
           <t>Ticket Médio Geral</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>250</v>
       </c>
     </row>
@@ -541,7 +544,7 @@
           <t>Faturamento Médio 3M</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>150000</v>
       </c>
     </row>
@@ -579,7 +582,7 @@
           <t>CAC</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>45</v>
       </c>
     </row>
@@ -589,7 +592,7 @@
           <t>Investimento Mkt</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -612,29 +615,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Categoria</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Periodo</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Faturamento</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Unidades</t>
         </is>
@@ -651,7 +654,7 @@
           <t>2025-01</t>
         </is>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>1000000</v>
       </c>
       <c r="D2" s="3" t="n">
@@ -669,7 +672,7 @@
           <t>2025-02</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>1100000</v>
       </c>
       <c r="D3" s="3" t="n">
@@ -687,7 +690,7 @@
           <t>2025-03</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>1050000</v>
       </c>
       <c r="D4" s="3" t="n">
@@ -705,7 +708,7 @@
           <t>2025-04</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>1200000</v>
       </c>
       <c r="D5" s="3" t="n">
@@ -723,7 +726,7 @@
           <t>2025-05</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>1150000</v>
       </c>
       <c r="D6" s="3" t="n">
@@ -741,7 +744,7 @@
           <t>2025-06</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>1300000</v>
       </c>
       <c r="D7" s="3" t="n">
@@ -775,27 +778,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Categoria_Macro</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Categoria Macro</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Subcategoria</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Periodo</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Faturamento</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Unidades</t>
         </is>
@@ -817,7 +820,7 @@
           <t>2025-01</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>500000</v>
       </c>
       <c r="E2" s="3" t="n">
@@ -840,7 +843,7 @@
           <t>2025-02</t>
         </is>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>550000</v>
       </c>
       <c r="E3" s="3" t="n">
@@ -863,7 +866,7 @@
           <t>2025-03</t>
         </is>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>520000</v>
       </c>
       <c r="E4" s="3" t="n">
@@ -886,7 +889,7 @@
           <t>2025-04</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>600000</v>
       </c>
       <c r="E5" s="3" t="n">
@@ -909,7 +912,7 @@
           <t>2025-05</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>580000</v>
       </c>
       <c r="E6" s="3" t="n">
@@ -932,7 +935,7 @@
           <t>2025-06</t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>650000</v>
       </c>
       <c r="E7" s="3" t="n">
@@ -955,7 +958,7 @@
           <t>2025-01</t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>200000</v>
       </c>
       <c r="E8" s="3" t="n">
@@ -978,7 +981,7 @@
           <t>2025-02</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>210000</v>
       </c>
       <c r="E9" s="3" t="n">
@@ -1001,7 +1004,7 @@
           <t>2025-03</t>
         </is>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>190000</v>
       </c>
       <c r="E10" s="3" t="n">
@@ -1024,7 +1027,7 @@
           <t>2025-04</t>
         </is>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>220000</v>
       </c>
       <c r="E11" s="3" t="n">
@@ -1047,7 +1050,7 @@
           <t>2025-05</t>
         </is>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>215000</v>
       </c>
       <c r="E12" s="3" t="n">
@@ -1070,7 +1073,7 @@
           <t>2025-06</t>
         </is>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>230000</v>
       </c>
       <c r="E13" s="3" t="n">

</xml_diff>